<commit_message>
small additions / restructuring
</commit_message>
<xml_diff>
--- a/kategoria_elemzes.xlsx
+++ b/kategoria_elemzes.xlsx
@@ -42,9 +42,6 @@
     <t>irányítás, koordináció, felelősség</t>
   </si>
   <si>
-    <t>külső vs. belső orientáció</t>
-  </si>
-  <si>
     <t>tények</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>státusz megszerzése</t>
   </si>
   <si>
-    <t>tudás, kihívások keresése</t>
-  </si>
-  <si>
     <t>konzervatív</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>elkülönülés vs. együttműködés</t>
+  </si>
+  <si>
+    <t>orientáció</t>
+  </si>
+  <si>
+    <t>tudás és kihívások keresése</t>
   </si>
 </sst>
 </file>
@@ -129,8 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,7 +437,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -442,9 +445,10 @@
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -458,87 +462,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1">
       <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:17">

</xml_diff>

<commit_message>
start coding the BOSCH material, add some text
</commit_message>
<xml_diff>
--- a/kategoria_elemzes.xlsx
+++ b/kategoria_elemzes.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>1. kiadvány</t>
-  </si>
-  <si>
-    <t>2. kiadvány</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>igazság alapja</t>
   </si>
@@ -94,6 +88,9 @@
   </si>
   <si>
     <t>tudás és kihívások keresése</t>
+  </si>
+  <si>
+    <t>Kiadvány kelte</t>
   </si>
 </sst>
 </file>
@@ -129,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -139,6 +136,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
@@ -455,108 +461,304 @@
     <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
     <col min="15" max="15" width="25.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="O1" s="4"/>
+      <c r="P1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1">
-      <c r="B2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>0</v>
+      <c r="A3" s="5">
+        <v>41391</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" t="s">
+      <c r="A4" s="5">
+        <v>41407</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="M4">
         <v>1</v>
       </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="5">
+        <v>41435</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="5">
+        <v>41486</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="5">
+        <v>41515</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="5">
+        <v>41536</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="5">
+        <v>41561</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="5">
+        <v>41589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="5">
+        <v>41618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="5">
+        <v>41668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="5">
+        <v>41698</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="5">
+        <v>41710</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="5">
+        <v>41759</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="5">
+        <v>41771</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="5">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="5">
+        <v>41834</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="5">
+        <v>41864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="5">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="5">
+        <v>41932</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="5">
+        <v>41953</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="5">
+        <v>42009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="5">
+        <v>42033</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="5">
+        <v>42059</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="5">
+        <v>42067</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="B1:C1"/>
@@ -566,7 +768,28 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B3:Q26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
finish coding the BOSCH material
</commit_message>
<xml_diff>
--- a/kategoria_elemzes.xlsx
+++ b/kategoria_elemzes.xlsx
@@ -54,12 +54,6 @@
     <t>innovatív</t>
   </si>
   <si>
-    <t>fókusz a feladaton</t>
-  </si>
-  <si>
-    <t>fókusz a kapcsolatokon</t>
-  </si>
-  <si>
     <t>egyéni</t>
   </si>
   <si>
@@ -87,17 +81,23 @@
     <t>orientáció</t>
   </si>
   <si>
-    <t>tudás és kihívások keresése</t>
-  </si>
-  <si>
     <t>Kiadvány kelte</t>
+  </si>
+  <si>
+    <t>feladat / eredmény fókusz</t>
+  </si>
+  <si>
+    <t>szociális / folyamat fókusz</t>
+  </si>
+  <si>
+    <t>tudás megszerz. kihívások keres.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +105,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,14 +138,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -145,6 +151,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,74 +456,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" customWidth="1"/>
     <col min="14" max="14" width="20.42578125" customWidth="1"/>
     <col min="15" max="15" width="25.28515625" customWidth="1"/>
-    <col min="16" max="16" width="7.7109375" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -522,7 +538,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>10</v>
@@ -530,33 +546,33 @@
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="5">
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
         <v>41391</v>
       </c>
       <c r="F3">
@@ -578,8 +594,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="5">
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
         <v>41407</v>
       </c>
       <c r="E4">
@@ -598,8 +614,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="5">
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
         <v>41435</v>
       </c>
       <c r="C5">
@@ -618,8 +634,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="5">
+    <row r="6" spans="1:19">
+      <c r="A6" s="3">
         <v>41486</v>
       </c>
       <c r="C6">
@@ -641,8 +657,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="5">
+    <row r="7" spans="1:19">
+      <c r="A7" s="3">
         <v>41515</v>
       </c>
       <c r="E7">
@@ -661,100 +677,374 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="5">
-        <v>41536</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="5">
+    <row r="8" spans="1:19">
+      <c r="A8" s="3">
+        <v>41537</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="3">
         <v>41561</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="5">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="3">
         <v>41589</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="5">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="3">
         <v>41618</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="5">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="3">
         <v>41668</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="5">
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="3">
         <v>41698</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="5">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="3">
         <v>41710</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="5">
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="3">
         <v>41759</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="5">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="3">
         <v>41771</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="5">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>4</v>
+      </c>
+      <c r="Q16">
+        <v>4</v>
+      </c>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="3">
         <v>41801</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="5">
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="6">
         <v>41834</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="5">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18" s="8"/>
+      <c r="S18" s="7"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="3">
         <v>41864</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="5">
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="3">
         <v>41905</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="5">
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="3">
         <v>41932</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="5">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>4</v>
+      </c>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="6">
         <v>41953</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="5">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" s="8"/>
+      <c r="S22" s="7"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="3">
         <v>42009</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="5">
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" s="3">
         <v>42033</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="5">
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="3">
         <v>42059</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="5">
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="3">
         <v>42067</v>
       </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -768,7 +1058,7 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:Q26">
+  <conditionalFormatting sqref="B3:Q26 Q27">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
not sure what changed, `status` says its the xls file, so committing the changes :D
</commit_message>
<xml_diff>
--- a/kategoria_elemzes.xlsx
+++ b/kategoria_elemzes.xlsx
@@ -494,15 +494,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>470648</xdr:colOff>
+      <xdr:colOff>470647</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>145677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>11205</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -812,7 +812,7 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add lots of stupid calculations
</commit_message>
<xml_diff>
--- a/kategoria_elemzes.xlsx
+++ b/kategoria_elemzes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>A</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>Σ említések</t>
   </si>
   <si>
     <t>kiadvány</t>
@@ -86,15 +83,44 @@
   <si>
     <t>teljesítményorientáció (E/a)</t>
   </si>
+  <si>
+    <t>Σ</t>
+  </si>
+  <si>
+    <t>variancia</t>
+  </si>
+  <si>
+    <t>említési arány</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -269,11 +295,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,43 +350,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -483,7 +540,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -812,7 +869,7 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -824,103 +881,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="22" t="s">
+      <c r="A1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="22" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="22" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="22" t="s">
+      <c r="M1" s="26"/>
+      <c r="N1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="22" t="s">
+      <c r="O1" s="26"/>
+      <c r="P1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="21"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="20"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="Q2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="21"/>
+      <c r="R2" s="20"/>
       <c r="U2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V2" s="1">
         <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>41391</v>
       </c>
       <c r="B3" s="8">
@@ -974,7 +1031,7 @@
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="15">
+      <c r="A4" s="14">
         <v>41407</v>
       </c>
       <c r="B4" s="11">
@@ -1028,7 +1085,7 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="15">
+      <c r="A5" s="14">
         <v>41435</v>
       </c>
       <c r="B5" s="11">
@@ -1082,7 +1139,7 @@
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="15">
+      <c r="A6" s="14">
         <v>41486</v>
       </c>
       <c r="B6" s="11">
@@ -1136,7 +1193,7 @@
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>41515</v>
       </c>
       <c r="B7" s="11">
@@ -1190,7 +1247,7 @@
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>41537</v>
       </c>
       <c r="B8" s="11">
@@ -1244,7 +1301,7 @@
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>41561</v>
       </c>
       <c r="B9" s="11">
@@ -1298,7 +1355,7 @@
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>41589</v>
       </c>
       <c r="B10" s="11">
@@ -1352,7 +1409,7 @@
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>41618</v>
       </c>
       <c r="B11" s="11">
@@ -1405,10 +1462,10 @@
       </c>
       <c r="R11" s="4"/>
       <c r="U11" t="s">
-        <v>15</v>
-      </c>
-      <c r="V11" s="25">
-        <f>W11/$V$2</f>
+        <v>14</v>
+      </c>
+      <c r="V11" s="22">
+        <f t="shared" ref="V11:V20" si="0">W11/$V$2</f>
         <v>0.171875</v>
       </c>
       <c r="W11">
@@ -1416,7 +1473,7 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="15">
+      <c r="A12" s="14">
         <v>41668</v>
       </c>
       <c r="B12" s="11">
@@ -1469,10 +1526,10 @@
       </c>
       <c r="R12" s="4"/>
       <c r="U12" t="s">
-        <v>14</v>
-      </c>
-      <c r="V12" s="25">
-        <f>W12/$V$2</f>
+        <v>13</v>
+      </c>
+      <c r="V12" s="22">
+        <f t="shared" si="0"/>
         <v>0.1484375</v>
       </c>
       <c r="W12">
@@ -1480,7 +1537,7 @@
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="15">
+      <c r="A13" s="14">
         <v>41698</v>
       </c>
       <c r="B13" s="11">
@@ -1533,10 +1590,10 @@
       </c>
       <c r="R13" s="4"/>
       <c r="U13" t="s">
-        <v>21</v>
-      </c>
-      <c r="V13" s="25">
-        <f>W13/$V$2</f>
+        <v>20</v>
+      </c>
+      <c r="V13" s="22">
+        <f t="shared" si="0"/>
         <v>0.12109375</v>
       </c>
       <c r="W13">
@@ -1544,7 +1601,7 @@
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="15">
+      <c r="A14" s="14">
         <v>41710</v>
       </c>
       <c r="B14" s="11">
@@ -1597,10 +1654,10 @@
       </c>
       <c r="R14" s="4"/>
       <c r="U14" t="s">
-        <v>22</v>
-      </c>
-      <c r="V14" s="25">
-        <f>W14/$V$2</f>
+        <v>21</v>
+      </c>
+      <c r="V14" s="22">
+        <f t="shared" si="0"/>
         <v>0.1171875</v>
       </c>
       <c r="W14">
@@ -1608,7 +1665,7 @@
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="15">
+      <c r="A15" s="14">
         <v>41759</v>
       </c>
       <c r="B15" s="11">
@@ -1662,10 +1719,10 @@
       <c r="R15" s="4"/>
       <c r="S15" s="3"/>
       <c r="U15" t="s">
-        <v>13</v>
-      </c>
-      <c r="V15" s="25">
-        <f>W15/$V$2</f>
+        <v>12</v>
+      </c>
+      <c r="V15" s="22">
+        <f t="shared" si="0"/>
         <v>0.1171875</v>
       </c>
       <c r="W15">
@@ -1673,7 +1730,7 @@
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="15">
+      <c r="A16" s="14">
         <v>41771</v>
       </c>
       <c r="B16" s="11">
@@ -1727,10 +1784,10 @@
       <c r="R16" s="4"/>
       <c r="S16" s="3"/>
       <c r="U16" t="s">
-        <v>16</v>
-      </c>
-      <c r="V16" s="25">
-        <f>W16/$V$2</f>
+        <v>15</v>
+      </c>
+      <c r="V16" s="22">
+        <f t="shared" si="0"/>
         <v>0.10546875</v>
       </c>
       <c r="W16">
@@ -1738,7 +1795,7 @@
       </c>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="15">
+      <c r="A17" s="14">
         <v>41801</v>
       </c>
       <c r="B17" s="11">
@@ -1792,10 +1849,10 @@
       <c r="R17" s="4"/>
       <c r="S17" s="3"/>
       <c r="U17" t="s">
-        <v>17</v>
-      </c>
-      <c r="V17" s="25">
-        <f>W17/$V$2</f>
+        <v>16</v>
+      </c>
+      <c r="V17" s="22">
+        <f t="shared" si="0"/>
         <v>8.59375E-2</v>
       </c>
       <c r="W17">
@@ -1803,7 +1860,7 @@
       </c>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="24">
+      <c r="A18" s="21">
         <v>41834</v>
       </c>
       <c r="B18" s="11">
@@ -1857,10 +1914,10 @@
       <c r="R18" s="4"/>
       <c r="S18" s="3"/>
       <c r="U18" t="s">
-        <v>18</v>
-      </c>
-      <c r="V18" s="25">
-        <f>W18/$V$2</f>
+        <v>17</v>
+      </c>
+      <c r="V18" s="22">
+        <f t="shared" si="0"/>
         <v>4.296875E-2</v>
       </c>
       <c r="W18">
@@ -1868,7 +1925,7 @@
       </c>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="15">
+      <c r="A19" s="14">
         <v>41864</v>
       </c>
       <c r="B19" s="11">
@@ -1922,10 +1979,10 @@
       <c r="R19" s="4"/>
       <c r="S19" s="3"/>
       <c r="U19" t="s">
-        <v>19</v>
-      </c>
-      <c r="V19" s="25">
-        <f>W19/$V$2</f>
+        <v>18</v>
+      </c>
+      <c r="V19" s="22">
+        <f t="shared" si="0"/>
         <v>3.90625E-2</v>
       </c>
       <c r="W19">
@@ -1933,7 +1990,7 @@
       </c>
     </row>
     <row r="20" spans="1:23">
-      <c r="A20" s="15">
+      <c r="A20" s="14">
         <v>41905</v>
       </c>
       <c r="B20" s="11">
@@ -1987,10 +2044,10 @@
       <c r="R20" s="4"/>
       <c r="S20" s="3"/>
       <c r="U20" t="s">
-        <v>12</v>
-      </c>
-      <c r="V20" s="25">
-        <f>W20/$V$2</f>
+        <v>11</v>
+      </c>
+      <c r="V20" s="22">
+        <f t="shared" si="0"/>
         <v>5.859375E-2</v>
       </c>
       <c r="W20">
@@ -1998,7 +2055,7 @@
       </c>
     </row>
     <row r="21" spans="1:23">
-      <c r="A21" s="15">
+      <c r="A21" s="14">
         <v>41932</v>
       </c>
       <c r="B21" s="11">
@@ -2053,7 +2110,7 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="1:23">
-      <c r="A22" s="24">
+      <c r="A22" s="21">
         <v>41953</v>
       </c>
       <c r="B22" s="11">
@@ -2108,7 +2165,7 @@
       <c r="S22" s="3"/>
     </row>
     <row r="23" spans="1:23">
-      <c r="A23" s="15">
+      <c r="A23" s="14">
         <v>42009</v>
       </c>
       <c r="B23" s="11">
@@ -2163,7 +2220,7 @@
       <c r="S23" s="3"/>
     </row>
     <row r="24" spans="1:23">
-      <c r="A24" s="15">
+      <c r="A24" s="14">
         <v>42033</v>
       </c>
       <c r="B24" s="11">
@@ -2218,7 +2275,7 @@
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="15">
+      <c r="A25" s="14">
         <v>42059</v>
       </c>
       <c r="B25" s="11">
@@ -2273,7 +2330,7 @@
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>42067</v>
       </c>
       <c r="B26" s="12">
@@ -2328,75 +2385,213 @@
       <c r="S26" s="3"/>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="9">
+        <f>SUM(B3:B26)</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="9">
+        <f t="shared" ref="C27:Q27" si="1">SUM(C3:C26)</f>
+        <v>3</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J27" s="9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K27" s="9">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B27" s="6">
-        <f>SUM(B3:B26)</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="6">
-        <f t="shared" ref="C27:Q27" si="0">SUM(C3:C26)</f>
+      <c r="L27" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N27" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="O27" s="9">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D27" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="6">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="F27" s="6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G27" s="6">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="H27" s="6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I27" s="6">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="J27" s="6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K27" s="6">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L27" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="6">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="N27" s="6">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O27" s="6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="P27" s="6">
-        <f t="shared" si="0"/>
+      <c r="P27" s="9">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="Q27" s="7">
-        <f t="shared" si="0"/>
+      <c r="Q27" s="10">
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="R27" s="20"/>
+      <c r="R27" s="19"/>
       <c r="S27" s="3"/>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="27">
+        <f>COUNTIF(B3:B26,"&gt;0")/24</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="27">
+        <f>COUNTIF(C3:C26,"&gt;0")/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D28" s="27">
+        <f>COUNTIF(D3:D26,"&gt;0")/24</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="27">
+        <f>COUNTIF(E3:E26,"&gt;0")/24</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F28" s="27">
+        <f>COUNTIF(F3:F26,"&gt;0")/24</f>
+        <v>0.625</v>
+      </c>
+      <c r="G28" s="27">
+        <f>COUNTIF(G3:G26,"&gt;0")/24</f>
+        <v>0.375</v>
+      </c>
+      <c r="H28" s="27">
+        <f>COUNTIF(H3:H26,"&gt;0")/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I28" s="27">
+        <f>COUNTIF(I3:I26,"&gt;0")/24</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="J28" s="27">
+        <f>COUNTIF(J3:J26,"&gt;0")/24</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K28" s="27">
+        <f>COUNTIF(K3:K26,"&gt;0")/24</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="L28" s="27">
+        <f>COUNTIF(L3:L26,"&gt;0")/24</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="27">
+        <f>COUNTIF(M3:M26,"&gt;0")/24</f>
+        <v>0.25</v>
+      </c>
+      <c r="N28" s="27">
+        <f>COUNTIF(N3:N26,"&gt;0")/24</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="O28" s="27">
+        <f>COUNTIF(O3:O26,"&gt;0")/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="P28" s="27">
+        <f>COUNTIF(P3:P26,"&gt;0")/24</f>
+        <v>0.375</v>
+      </c>
+      <c r="Q28" s="28">
+        <f>COUNTIF(Q3:Q26,"&gt;0")/24</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="30">
+        <f>VAR(B3:B26)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="30">
+        <f>VAR(C3:C26)</f>
+        <v>0.20108695652173914</v>
+      </c>
+      <c r="D29" s="30">
+        <f>VAR(D3:D26)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="30">
+        <f>VAR(E3:E26)</f>
+        <v>2.3025362318840581</v>
+      </c>
+      <c r="F29" s="30">
+        <f>VAR(F3:F26)</f>
+        <v>1.7608695652173914</v>
+      </c>
+      <c r="G29" s="29">
+        <f>VAR(G3:G26)</f>
+        <v>3.2445652173913042</v>
+      </c>
+      <c r="H29" s="30">
+        <f>VAR(H3:H26)</f>
+        <v>0.20108695652173914</v>
+      </c>
+      <c r="I29" s="29">
+        <f>VAR(I3:I26)</f>
+        <v>4.4057971014492754</v>
+      </c>
+      <c r="J29" s="29">
+        <f>VAR(J3:J26)</f>
+        <v>3.3260869565217392</v>
+      </c>
+      <c r="K29" s="30">
+        <f>VAR(K3:K26)</f>
+        <v>0.86231884057971009</v>
+      </c>
+      <c r="L29" s="30">
+        <f>VAR(L3:L26)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="30">
+        <f>VAR(M3:M26)</f>
+        <v>0.95471014492753614</v>
+      </c>
+      <c r="N29" s="30">
+        <f>VAR(N3:N26)</f>
+        <v>0.28260869565217389</v>
+      </c>
+      <c r="O29" s="30">
+        <f>VAR(O3:O26)</f>
+        <v>0.20108695652173914</v>
+      </c>
+      <c r="P29" s="30">
+        <f>VAR(P3:P26)</f>
+        <v>1.9927536231884055</v>
+      </c>
+      <c r="Q29" s="31">
+        <f>VAR(Q3:Q26)</f>
+        <v>2.6014492753623188</v>
+      </c>
     </row>
     <row r="32" spans="1:23">
       <c r="B32">
@@ -2465,7 +2660,7 @@
     <mergeCell ref="L1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:Q26">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -2473,7 +2668,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2485,12 +2680,40 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:Q27">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
         <color rgb="FFFFEF9C"/>
         <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:Q28">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:Q29">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <color theme="8" tint="0.59999389629810485"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>